<commit_message>
Dodani plovi in članstvo za Velikonočno
</commit_message>
<xml_diff>
--- a/podatki/sv.Nikola/nikola_jadralci.xlsx
+++ b/podatki/sv.Nikola/nikola_jadralci.xlsx
@@ -4982,7 +4982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K412"/>
   <sheetViews>
-    <sheetView topLeftCell="A380" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H380" sqref="H380"/>
     </sheetView>
   </sheetViews>
@@ -17362,8 +17362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A377" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17393,8 +17393,8 @@
         <v xml:space="preserve"> SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'CRO1202') t;</v>
       </c>
       <c r="E1" t="str">
-        <f>CONCATENATE(" WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec FROM clanstvo WHERE sailno = ",D1,");")</f>
-        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec FROM clanstvo WHERE sailno =  SELECT idtekmovalec FROM tekmovalec WHERE sailno = 'CRO1202') t;);</v>
+        <f>CONCATENATE(" WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec FROM clanstvo JOIN tekmovalec on idtekmovalec = tekmovalec_idtekmovalec);")</f>
+        <v xml:space="preserve"> WHERE NOT EXISTS (SELECT tekmovalec_idtekmovalec, idtekmovalec FROM clanstvo JOIN tekmovalec on idtekmovalec = tekmovalec_idtekmovalec);</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>

</xml_diff>